<commit_message>
Modifying the COursesInputTemplate and the Courses input files for the exisiting problem instances
</commit_message>
<xml_diff>
--- a/ifs-solver/src/main/resources/CoursesInputTemplate.xlsx
+++ b/ifs-solver/src/main/resources/CoursesInputTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talha\Documents\CS Honours\COMP700 - HP\student-lab-sectioning\ifs-solver\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00890781-E5AC-4583-B708-9A6C29703BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708BD36A-0FB0-4BEB-B289-4759F2FE2F76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,16 +36,16 @@
     <t>sectionNum</t>
   </si>
   <si>
-    <t>allocatedDay</t>
-  </si>
-  <si>
-    <t>allocatedTimeslot</t>
-  </si>
-  <si>
     <t>sessionLength</t>
   </si>
   <si>
     <t>venueCapacity</t>
+  </si>
+  <si>
+    <t>sessionDay</t>
+  </si>
+  <si>
+    <t>sessionStartTime</t>
   </si>
 </sst>
 </file>
@@ -363,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,21 +382,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G2">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>